<commit_message>
[WIP] Add failing tests for Antibody Results import
CVDLS-201
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
+++ b/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDD84C6-04FD-4C47-B2B3-05CE2A0F2750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D986C4-1CC2-584F-9232-CD9CCA843F5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="4540" windowWidth="21780" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="4540" windowWidth="24280" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="G900153336_calls" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>Specimen ID</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>G814450905</t>
-  </si>
-  <si>
-    <t>C04</t>
   </si>
   <si>
     <t>C05</t>
@@ -296,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,6 +471,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -638,9 +647,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -997,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1046,25 +1057,25 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H2" t="s">
@@ -1075,25 +1086,25 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H3" t="s">
@@ -1107,25 +1118,23 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H5" t="s">
@@ -1136,94 +1145,112 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
+      <c r="A7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
+      <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3"/>
       <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I10" s="1"/>
@@ -1284,6 +1311,9 @@
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I30" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
Antibody Results Import now better covers error cases with tests
CVDLS-201
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
+++ b/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D986C4-1CC2-584F-9232-CD9CCA843F5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A44DD4-256E-604F-82C2-F3316754C2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="4540" windowWidth="24280" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1011,7 +1011,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Antibody Import Test adds test for Non-Negative result
CVDLS-201
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
+++ b/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A44DD4-256E-604F-82C2-F3316754C2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC4DFE5-BEA5-7042-9C66-29C88ABCA7A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="4540" windowWidth="24280" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Specimen ID</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t>SpecimenAntibodyResults6</t>
+  </si>
+  <si>
+    <t>SpecimenAntibodyResults7</t>
+  </si>
+  <si>
+    <t>G814450907</t>
+  </si>
+  <si>
+    <t>Non-Negative</t>
+  </si>
+  <si>
+    <t>C07</t>
   </si>
 </sst>
 </file>
@@ -1008,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1115,40 +1127,42 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2" t="s">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1173,17 +1187,17 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -1192,26 +1206,26 @@
         <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="2">
-        <v>3</v>
-      </c>
-      <c r="E8" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
@@ -1219,41 +1233,65 @@
         <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I11" s="1"/>
@@ -1314,6 +1352,9 @@
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I31" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
Antibody Results test verifies mismatched Well Position throws error
CVDLS-201
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
+++ b/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC4DFE5-BEA5-7042-9C66-29C88ABCA7A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E216427A-AAB5-8D44-BDDC-8584D97B5115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="4540" windowWidth="24280" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>Specimen ID</t>
   </si>
@@ -56,15 +56,9 @@
     <t>Positive</t>
   </si>
   <si>
-    <t>Data Links</t>
-  </si>
-  <si>
     <t>Signal</t>
   </si>
   <si>
-    <t>20200617_1</t>
-  </si>
-  <si>
     <t>Storage Rack</t>
   </si>
   <si>
@@ -150,6 +144,45 @@
   </si>
   <si>
     <t>C07</t>
+  </si>
+  <si>
+    <t>SpecimenAntibodyResults8</t>
+  </si>
+  <si>
+    <t>Data Links (but used for Comments here)</t>
+  </si>
+  <si>
+    <t>Verify Negative conclusion</t>
+  </si>
+  <si>
+    <t>Verify Positive conclusion</t>
+  </si>
+  <si>
+    <t>Verify Non-Negative conclusion</t>
+  </si>
+  <si>
+    <t>Verify error on missing Specimen ID</t>
+  </si>
+  <si>
+    <t>Verify error on missing Biobank Tube ID</t>
+  </si>
+  <si>
+    <t>Verify error on missing Conclusion</t>
+  </si>
+  <si>
+    <t>Verify error on missing Well Position</t>
+  </si>
+  <si>
+    <t>Verify error on missing Well Plate Barcode</t>
+  </si>
+  <si>
+    <t>Verify error when uploaded result Well Position doesn't match</t>
+  </si>
+  <si>
+    <t>H10</t>
+  </si>
+  <si>
+    <t>G814450908</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1056,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1033,7 +1066,7 @@
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="5.5" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="50.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.1640625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" customWidth="1"/>
@@ -1044,36 +1077,36 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -1085,24 +1118,24 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -1114,45 +1147,45 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="D4" s="2">
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1161,7 +1194,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
@@ -1173,21 +1206,21 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="2" t="s">
@@ -1200,24 +1233,24 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2">
@@ -1227,24 +1260,24 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -1254,24 +1287,24 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
@@ -1280,21 +1313,47 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I11" s="1"/>
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I12" s="1"/>

</xml_diff>

<commit_message>
Antibody Results test verifies Well ID must match
CVDLS-201
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
+++ b/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E216427A-AAB5-8D44-BDDC-8584D97B5115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F491C7-60FD-EF42-96A6-AF9A98C27620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="4540" windowWidth="24280" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>Specimen ID</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>G814450908</t>
+  </si>
+  <si>
+    <t>SpecimenAntibodyResults9</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>Verify error when uploaded result Well ID doesn't match</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1065,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1356,7 +1365,33 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I12" s="1"/>
+      <c r="A12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5555555</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I13" s="1"/>

</xml_diff>

<commit_message>
CVDLS-296 Added handling of result conclusion "REJECTED"
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
+++ b/tests/ExcelImport/workbooks/specimen-antibody-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abk/Projects/covid/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F491C7-60FD-EF42-96A6-AF9A98C27620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9986797E-A46C-DE4C-9AF1-E947692709F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="4540" windowWidth="24280" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="4540" windowWidth="41420" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="G900153336_calls" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <t>Specimen ID</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>Verify error when uploaded result Well ID doesn't match</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Verify that rejected specimen's status is updated and has no result created</t>
+  </si>
+  <si>
+    <t>SpecimenAntibodyResults10</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1074,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1075,7 +1084,7 @@
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="5.5" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="65.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.1640625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" customWidth="1"/>
@@ -1394,6 +1403,18 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1453,5 +1474,6 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>